<commit_message>
add age structure, unsure if working
</commit_message>
<xml_diff>
--- a/tests/test_data/south_africa_age_data.xlsx
+++ b/tests/test_data/south_africa_age_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/hpvsim/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438A0348-6E6A-6640-AE5C-B37308AC4450}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE81852-A394-074C-B47A-20A4D77B8BEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15560" xr2:uid="{5D7E3FBA-9D2B-2843-BAA4-D4EB28E49B52}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -405,13 +405,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C9993B8-80AA-8549-899C-308C8A5037BC}">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2001</v>
       </c>
@@ -451,7 +454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -472,7 +475,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2001</v>
       </c>
@@ -493,7 +496,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -514,7 +517,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2001</v>
       </c>
@@ -535,7 +538,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2001</v>
       </c>
@@ -556,7 +559,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2001</v>
       </c>
@@ -577,7 +580,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2001</v>
       </c>
@@ -598,7 +601,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2002</v>
       </c>
@@ -618,7 +621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2002</v>
       </c>
@@ -639,7 +642,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2002</v>
       </c>
@@ -660,7 +663,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2002</v>
       </c>
@@ -681,7 +684,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2002</v>
       </c>
@@ -702,7 +705,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -723,7 +726,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2002</v>
       </c>
@@ -744,7 +747,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2002</v>
       </c>
@@ -765,7 +768,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2003</v>
       </c>
@@ -785,7 +788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2003</v>
       </c>
@@ -806,7 +809,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2003</v>
       </c>
@@ -827,7 +830,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2003</v>
       </c>
@@ -848,7 +851,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2003</v>
       </c>
@@ -869,7 +872,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2003</v>
       </c>
@@ -890,7 +893,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2003</v>
       </c>
@@ -911,7 +914,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -932,7 +935,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -952,7 +955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2004</v>
       </c>
@@ -973,7 +976,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2004</v>
       </c>
@@ -994,7 +997,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2004</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2004</v>
       </c>
@@ -1036,7 +1039,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2004</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2004</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2004</v>
       </c>
@@ -1099,7 +1102,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2005</v>
       </c>
@@ -1119,7 +1122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2005</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2005</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2005</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2005</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2005</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2005</v>
       </c>
@@ -1245,7 +1248,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2005</v>
       </c>
@@ -1266,7 +1269,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2006</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2006</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2006</v>
       </c>
@@ -1328,7 +1331,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2006</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2006</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2006</v>
       </c>
@@ -1391,7 +1394,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2006</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2006</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2007</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2007</v>
       </c>
@@ -1474,7 +1477,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2007</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2007</v>
       </c>
@@ -1516,7 +1519,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2007</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2007</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2007</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2007</v>
       </c>
@@ -1600,7 +1603,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2008</v>
       </c>
@@ -1620,7 +1623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2008</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2008</v>
       </c>
@@ -1662,7 +1665,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2008</v>
       </c>
@@ -1683,7 +1686,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2008</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2008</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>886</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2008</v>
       </c>
@@ -1746,7 +1749,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2009</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2009</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2009</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2009</v>
       </c>
@@ -1850,7 +1853,7 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2009</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2009</v>
       </c>
@@ -1892,7 +1895,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2009</v>
       </c>
@@ -1913,7 +1916,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2009</v>
       </c>
@@ -1934,7 +1937,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2010</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2010</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2010</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2010</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2010</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2010</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2010</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2010</v>
       </c>
@@ -2101,7 +2104,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2011</v>
       </c>
@@ -2121,7 +2124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2011</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2011</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2011</v>
       </c>
@@ -2184,7 +2187,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2011</v>
       </c>
@@ -2205,7 +2208,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2011</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2011</v>
       </c>
@@ -2247,7 +2250,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2011</v>
       </c>
@@ -2268,7 +2271,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2012</v>
       </c>
@@ -2288,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2012</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2012</v>
       </c>
@@ -2330,7 +2333,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2012</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2012</v>
       </c>
@@ -2372,7 +2375,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2012</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2012</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2012</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2013</v>
       </c>
@@ -2455,7 +2458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2013</v>
       </c>
@@ -2476,7 +2479,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2013</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2013</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2013</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2013</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2013</v>
       </c>
@@ -2581,7 +2584,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2013</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2014</v>
       </c>
@@ -2622,7 +2625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2014</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2014</v>
       </c>
@@ -2664,7 +2667,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2014</v>
       </c>
@@ -2685,7 +2688,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2014</v>
       </c>
@@ -2706,7 +2709,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2014</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2014</v>
       </c>
@@ -2748,7 +2751,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2014</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2015</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2015</v>
       </c>
@@ -2810,7 +2813,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2015</v>
       </c>
@@ -2831,7 +2834,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2015</v>
       </c>
@@ -2852,7 +2855,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2015</v>
       </c>
@@ -2873,7 +2876,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2015</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2015</v>
       </c>
@@ -2915,7 +2918,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="121" spans="1:6">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2015</v>
       </c>
@@ -2935,7 +2938,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2016</v>
       </c>
@@ -2955,7 +2958,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:6">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>2016</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2016</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2016</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2016</v>
       </c>
@@ -3039,7 +3042,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2016</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="128" spans="1:6">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2016</v>
       </c>
@@ -3081,7 +3084,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2016</v>
       </c>
@@ -3101,7 +3104,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2017</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:6">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2017</v>
       </c>
@@ -3143,7 +3146,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2017</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="133" spans="1:6">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2017</v>
       </c>
@@ -3185,7 +3188,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="134" spans="1:6">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>2017</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="135" spans="1:6">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2017</v>
       </c>
@@ -3227,7 +3230,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2017</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2017</v>
       </c>
@@ -3268,7 +3271,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2018</v>
       </c>
@@ -3288,7 +3291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2018</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2018</v>
       </c>
@@ -3330,7 +3333,7 @@
         <v>1207</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2018</v>
       </c>
@@ -3351,7 +3354,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2018</v>
       </c>
@@ -3372,7 +3375,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2018</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2018</v>
       </c>
@@ -3414,7 +3417,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2018</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2019</v>
       </c>
@@ -3455,7 +3458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2019</v>
       </c>
@@ -3476,7 +3479,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2019</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2019</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>2059</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2019</v>
       </c>
@@ -3539,7 +3542,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2019</v>
       </c>
@@ -3560,7 +3563,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2019</v>
       </c>
@@ -3581,7 +3584,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2019</v>
       </c>

</xml_diff>